<commit_message>
completed edit Revision page object locators
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_FASB.xlsx
+++ b/src/main/resources/objectLocator/OR_FASB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\objectLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9A74AB-46BE-47B9-8743-7A9CE28EE2C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E7BCB7-46FF-4E2D-9691-39B97A21F994}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIGeneric" sheetId="38" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="169">
   <si>
     <t>panelExportWidgetHeader</t>
   </si>
@@ -242,6 +242,303 @@
   </si>
   <si>
     <t>Parent</t>
+  </si>
+  <si>
+    <t>//*[@id="tbarCmdEdit"]</t>
+  </si>
+  <si>
+    <t>btnEdit</t>
+  </si>
+  <si>
+    <t>panelEditRevision</t>
+  </si>
+  <si>
+    <t>//*[@id="wndEditRevisions"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ResidualValueGuarantee"]</t>
+  </si>
+  <si>
+    <t>txtRVG</t>
+  </si>
+  <si>
+    <t>//*[@id="FMVOfLease"]</t>
+  </si>
+  <si>
+    <t>txtFMV</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="HasPurchaseOption_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="IsOwnershipTransferAtEndOfLease_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="IsNPVMoreThanFMV_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="IsLeaseEncompassingUsefulLife_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='IsSpecializedAsset_listbox']</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='CollectPayment_listbox']</t>
+  </si>
+  <si>
+    <t>question1</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>question3</t>
+  </si>
+  <si>
+    <t>question4</t>
+  </si>
+  <si>
+    <t>question5</t>
+  </si>
+  <si>
+    <t>question6</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='isThirdPartyMoreThanFMV_listbox']</t>
+  </si>
+  <si>
+    <t>question7</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='FASBClassificationTypeID_listbox']</t>
+  </si>
+  <si>
+    <t>dpLeaseClasification</t>
+  </si>
+  <si>
+    <t>txtUsefulLife</t>
+  </si>
+  <si>
+    <t>//*[@id="UsefulLife"]</t>
+  </si>
+  <si>
+    <t>txtCalender</t>
+  </si>
+  <si>
+    <t>//*[@id="RevisionCalendar"]</t>
+  </si>
+  <si>
+    <t>txtPaymentType</t>
+  </si>
+  <si>
+    <t>//*[@id="RevisionChargeId"]</t>
+  </si>
+  <si>
+    <t>//*[@id="IndexIncluded"]</t>
+  </si>
+  <si>
+    <t>//*[@id="Index_Rate"]</t>
+  </si>
+  <si>
+    <t>txtIndexRate</t>
+  </si>
+  <si>
+    <t>//*[@id="Fixed_Monthly_Index_Rent"]</t>
+  </si>
+  <si>
+    <t>//*[@id="Total_Index_Rent"]</t>
+  </si>
+  <si>
+    <t>txtIndexRent</t>
+  </si>
+  <si>
+    <t>txtMonthlyIndexRent</t>
+  </si>
+  <si>
+    <t>//*[@id="TotalMonthlyAmount"]</t>
+  </si>
+  <si>
+    <t>txtTotalPeriodPayments</t>
+  </si>
+  <si>
+    <t>//*[@id="TotalAmountCapitalized"]</t>
+  </si>
+  <si>
+    <t>txtTotalAmountCapitalize</t>
+  </si>
+  <si>
+    <t>//*[@id="ServiceRentType"]</t>
+  </si>
+  <si>
+    <t>dpServiceRentType</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="NPVInterestRateId_listbox"]</t>
+  </si>
+  <si>
+    <t>dpInterestRateTerm</t>
+  </si>
+  <si>
+    <t>//*[@id="NPVInterestRateOfInterest"]</t>
+  </si>
+  <si>
+    <t>txtClientInterestRate</t>
+  </si>
+  <si>
+    <t>//*[@id="LeaseLiabilityROUBase"]</t>
+  </si>
+  <si>
+    <t>txtLeaseLiabilityROUBase</t>
+  </si>
+  <si>
+    <t>//*[@id="Prepayment"]</t>
+  </si>
+  <si>
+    <t>txtPrepayment</t>
+  </si>
+  <si>
+    <t>//*[@id="ROU_InitialDirectCosts"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ROU_LandlordAllowance"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ROU_ImpairmentsAsset"]</t>
+  </si>
+  <si>
+    <t>txtROU_InitialDirectCosts</t>
+  </si>
+  <si>
+    <t>txtROU_LandlordAllowance</t>
+  </si>
+  <si>
+    <t>txtROU_ImpairmentsAsset</t>
+  </si>
+  <si>
+    <t>//*[@id="ROU_LeaseIncentive"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ROU_TotalAssetBalance"]</t>
+  </si>
+  <si>
+    <t>txtROU_LeaseIncentive</t>
+  </si>
+  <si>
+    <t>txtROU_TotalAssetBalance</t>
+  </si>
+  <si>
+    <t>cbIncludeIndex</t>
+  </si>
+  <si>
+    <t>cbIndexRate</t>
+  </si>
+  <si>
+    <t>btnAddNew</t>
+  </si>
+  <si>
+    <t>//*[@id="btnAddNew"]</t>
+  </si>
+  <si>
+    <t>btnDelete</t>
+  </si>
+  <si>
+    <t>//*[@id="btnDelete"]</t>
+  </si>
+  <si>
+    <t>buttonDelete</t>
+  </si>
+  <si>
+    <t>//*[@id="buttonDelete"]</t>
+  </si>
+  <si>
+    <t>btnSave</t>
+  </si>
+  <si>
+    <t>//*[@id="btnSave"]</t>
+  </si>
+  <si>
+    <t>btnClose</t>
+  </si>
+  <si>
+    <t>//*[@id="EditRevisionPopUpClose"]</t>
+  </si>
+  <si>
+    <t>txtAccruedBal</t>
+  </si>
+  <si>
+    <t>//*[@id="PreviousRevAccruedBal"]</t>
+  </si>
+  <si>
+    <t>txtW/OAmt</t>
+  </si>
+  <si>
+    <t>//*[@id="Prior_Rev_WO_Amt"]</t>
+  </si>
+  <si>
+    <t>txtAccruedBeginningBalance</t>
+  </si>
+  <si>
+    <t>//*[@id="Prior_Rev_RollOver_Amt"]</t>
+  </si>
+  <si>
+    <t>level_pname</t>
+  </si>
+  <si>
+    <t>//*[@id="aPropName"]</t>
+  </si>
+  <si>
+    <t>level_lname</t>
+  </si>
+  <si>
+    <t>//*[@id="aLeaseName"]</t>
+  </si>
+  <si>
+    <t>level_revisionNumber</t>
+  </si>
+  <si>
+    <t>//*[@id="revisionNumber"]</t>
+  </si>
+  <si>
+    <t>level_RevisionDesc</t>
+  </si>
+  <si>
+    <t>//*[@id="RevisionDesc"]</t>
+  </si>
+  <si>
+    <t>level_RevisionDate</t>
+  </si>
+  <si>
+    <t>//*[@id="RevisionDate"]</t>
+  </si>
+  <si>
+    <t>level_RevAdj13Period</t>
+  </si>
+  <si>
+    <t>//*[@id="RevAdj13Period"]</t>
+  </si>
+  <si>
+    <t>ck_PartialTermination</t>
+  </si>
+  <si>
+    <t>//*[@id="PartialTermination"]</t>
+  </si>
+  <si>
+    <t>level_FASB/IASBStartDate</t>
+  </si>
+  <si>
+    <t>//*[@id="Start"]</t>
+  </si>
+  <si>
+    <t>level_FASB/IASBEndDate</t>
+  </si>
+  <si>
+    <t>//*[@id="End"]</t>
+  </si>
+  <si>
+    <t>level_tdPeriods</t>
+  </si>
+  <si>
+    <t>//*[@id="tdPeriods"]</t>
   </si>
 </sst>
 </file>
@@ -320,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -343,11 +640,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,41 +693,17 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1572,19 +1856,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="78" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="77" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="76" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="75" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1593,17 +1877,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" customWidth="1"/>
   </cols>
@@ -1689,21 +1973,573 @@
         <v>33</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>165</v>
+      </c>
+      <c r="B57" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A7 A150:A1048576">
-    <cfRule type="duplicateValues" dxfId="73" priority="73"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A7 A150:A1048576">
-    <cfRule type="duplicateValues" dxfId="72" priority="77"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A7 A150:A1048576">
-    <cfRule type="duplicateValues" dxfId="71" priority="79"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A7 A150:A1048576">
-    <cfRule type="duplicateValues" dxfId="70" priority="85"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A150:A1048576 A1:A7">
-    <cfRule type="duplicateValues" dxfId="69" priority="87"/>
+  <conditionalFormatting sqref="A151:A1048576 A1:A34 A37:A38">
+    <cfRule type="duplicateValues" dxfId="70" priority="73"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A151:A1048576">
+    <cfRule type="duplicateValues" dxfId="69" priority="77"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1716,7 +2552,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>

</xml_diff>

<commit_message>
Add: Sxript for update revision
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_FASB.xlsx
+++ b/src/main/resources/objectLocator/OR_FASB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\objectLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189548EB-B875-4FDB-BF48-15A1C6F06FEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890BD335-3B43-4787-9FE0-5A197E185ADC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIGeneric" sheetId="38" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="187">
   <si>
     <t>panelExportWidgetHeader</t>
   </si>
@@ -469,9 +469,6 @@
     <t>txtAccruedBeginningBalance</t>
   </si>
   <si>
-    <t>//*[@id="Prior_Rev_RollOver_Amt"]</t>
-  </si>
-  <si>
     <t>level_pname</t>
   </si>
   <si>
@@ -575,6 +572,27 @@
   </si>
   <si>
     <t>txtNotes</t>
+  </si>
+  <si>
+    <t>AccruedBeginningBalance</t>
+  </si>
+  <si>
+    <t>FMVOfLease</t>
+  </si>
+  <si>
+    <t>//*[@name="ResidualValueGuarantee"]</t>
+  </si>
+  <si>
+    <t>txtUnguaranteedResidualValue</t>
+  </si>
+  <si>
+    <t>UnguaranteedResidualValue</t>
+  </si>
+  <si>
+    <t>txtCarryingAmountofAssets</t>
+  </si>
+  <si>
+    <t>CarryingAmountofAssets</t>
   </si>
 </sst>
 </file>
@@ -1913,11 +1931,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2054,7 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2050,7 +2068,7 @@
         <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,7 +2104,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2100,7 +2118,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,7 +2132,7 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2128,7 +2146,7 @@
         <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2330,7 @@
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -2323,7 +2341,7 @@
         <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -2334,7 +2352,7 @@
         <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
@@ -2473,11 +2491,11 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>144</v>
+      <c r="A48" t="s">
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -2485,10 +2503,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C49" t="s">
         <v>37</v>
@@ -2496,10 +2514,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C50" t="s">
         <v>37</v>
@@ -2507,10 +2525,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
@@ -2518,10 +2536,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
         <v>37</v>
@@ -2529,10 +2547,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C53" t="s">
         <v>37</v>
@@ -2540,10 +2558,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C54" t="s">
         <v>37</v>
@@ -2551,10 +2569,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s">
         <v>37</v>
@@ -2562,10 +2580,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
@@ -2573,10 +2591,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
         <v>37</v>
@@ -2584,13 +2602,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
+      </c>
+      <c r="E58" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2598,42 +2619,83 @@
         <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C59" t="s">
         <v>37</v>
-      </c>
-      <c r="E59" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>171</v>
-      </c>
-      <c r="B60" t="s">
-        <v>169</v>
+        <v>179</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="C61" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A151:A1048576 A1:A34 A37:A38">
+  <conditionalFormatting sqref="A150:A1048576 A1:A34 A37:A38">
     <cfRule type="duplicateValues" dxfId="70" priority="73"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:A1048576">
+  <conditionalFormatting sqref="A150:A1048576">
     <cfRule type="duplicateValues" dxfId="69" priority="77"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Partial Script for add revision
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_FASB.xlsx
+++ b/src/main/resources/objectLocator/OR_FASB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\objectLocator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSI\AMTAutomationRipo\AMT-TestFrameWork\src\main\resources\objectLocator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26687E65-E52E-4387-B754-C1A95B2306AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4575" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="5025" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FIGeneric" sheetId="38" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="221">
   <si>
     <t>panelExportWidgetHeader</t>
   </si>
@@ -689,12 +688,18 @@
   </si>
   <si>
     <t>txtTotalIndexRent</t>
+  </si>
+  <si>
+    <t>dpSpace</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='RevisionSuiteIndexId_listbox']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1899,7 +1904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2036,12 +2041,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD82"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,7 +2979,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>216</v>
       </c>
@@ -2985,7 +2990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>218</v>
       </c>
@@ -2994,6 +2999,20 @@
       </c>
       <c r="C82" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>219</v>
+      </c>
+      <c r="B83" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" t="s">
+        <v>37</v>
+      </c>
+      <c r="E83" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3004,7 +3023,7 @@
     <cfRule type="duplicateValues" dxfId="70" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3012,7 +3031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3210,190 +3229,190 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:A1048576 A2 A7">
-    <cfRule type="duplicateValues" dxfId="69" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="duplicateValues" dxfId="68" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="duplicateValues" dxfId="67" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="duplicateValues" dxfId="66" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="duplicateValues" dxfId="65" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="64" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="63" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="62" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="61" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="60" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="59" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="58" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="57" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="56" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="55" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="54" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="53" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="52" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="51" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="50" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="49" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="48" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="47" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="46" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="45" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="44" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="43" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="42" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="41" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="40" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="39" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="38" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="37" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="36" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="35" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="34" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="33" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="32" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="31" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="30" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="29" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="28" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="27" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="26" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="25" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="23" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="22" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="21" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="20" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="17" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="16" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3401,12 +3420,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,27 +3552,27 @@
       <c r="E5" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A4" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:A4"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="7" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A1048576 A1:A3">
-    <cfRule type="duplicateValues" dxfId="3" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="72"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Work for post revision test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_FASB.xlsx
+++ b/src/main/resources/objectLocator/OR_FASB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="5475" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="6375" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FIGeneric" sheetId="38" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="241">
   <si>
     <t>panelExportWidgetHeader</t>
   </si>
@@ -700,13 +700,67 @@
   </si>
   <si>
     <t>//*[contains(@id,'RENTABLE_SQFT')]</t>
+  </si>
+  <si>
+    <t>tbarCmdPrint_report</t>
+  </si>
+  <si>
+    <t>btnPrint</t>
+  </si>
+  <si>
+    <t>tbarCmdreport_cancel</t>
+  </si>
+  <si>
+    <t>btnCancel</t>
+  </si>
+  <si>
+    <t>processCount</t>
+  </si>
+  <si>
+    <t>//*[@id='pin']</t>
+  </si>
+  <si>
+    <t>queueCount</t>
+  </si>
+  <si>
+    <t>//*[@class='sub-title']</t>
+  </si>
+  <si>
+    <t>tbarCmdPost</t>
+  </si>
+  <si>
+    <t>btnPost</t>
+  </si>
+  <si>
+    <t>tbarCmdTransaction_report</t>
+  </si>
+  <si>
+    <t>btnTransactionReport</t>
+  </si>
+  <si>
+    <t>tbarCmdJournalEntry</t>
+  </si>
+  <si>
+    <t>btnJEReport</t>
+  </si>
+  <si>
+    <t>tbarCmdFxJournalEntry</t>
+  </si>
+  <si>
+    <t>btnFXJEReport</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),"Save")]</t>
+  </si>
+  <si>
+    <t>tbBatchHistroy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +798,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF808080"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -816,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,6 +919,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2050,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
     </sheetView>
@@ -3049,18 +3112,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="2" max="3" width="47" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="56.5703125" customWidth="1"/>
   </cols>
@@ -3244,20 +3306,133 @@
         <v>37</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:A1048576 A2 A7">
+  <conditionalFormatting sqref="A15:A17 A2 A7 A20:A1048576">
     <cfRule type="duplicateValues" dxfId="68" priority="65"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A1048576">
+  <conditionalFormatting sqref="A15:A17 A20:A1048576">
     <cfRule type="duplicateValues" dxfId="67" priority="64"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A1048576">
+  <conditionalFormatting sqref="A15:A17 A20:A1048576">
     <cfRule type="duplicateValues" dxfId="66" priority="63"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A1048576">
+  <conditionalFormatting sqref="A15:A17 A20:A1048576">
     <cfRule type="duplicateValues" dxfId="65" priority="62"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A1048576">
+  <conditionalFormatting sqref="A15:A17 A20:A1048576">
     <cfRule type="duplicateValues" dxfId="64" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">

</xml_diff>

<commit_message>
Work for 54 Smoke test cases in App env
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_FASB.xlsx
+++ b/src/main/resources/objectLocator/OR_FASB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6375" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="7275" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FIGeneric" sheetId="38" r:id="rId1"/>
@@ -2113,9 +2113,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,9 +3114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>